<commit_message>
Entra a SCT, saca la deuda y genera un Excel final
</commit_message>
<xml_diff>
--- a/Data/Clientes.xlsx
+++ b/Data/Clientes.xlsx
@@ -951,7 +951,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Error volver a iniciar sesion</t>
+          <t>Error autenticacion</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Error volver a iniciar sesion</t>
+          <t>Error autenticacion</t>
         </is>
       </c>
     </row>
@@ -1297,11 +1297,7 @@
       <c r="F30" t="n">
         <v>0</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Error autenticacion</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1498,7 +1494,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>No contiene 351</t>
+          <t>Error autenticacion</t>
         </is>
       </c>
     </row>
@@ -1672,7 +1668,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Error volver a iniciar sesion</t>
+          <t>Error autenticacion</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1944,11 @@
       <c r="F53" t="n">
         <v>1</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Error autenticacion</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2197,11 +2197,7 @@
       <c r="F62" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Error autenticacion</t>
-        </is>
-      </c>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2253,7 +2249,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Error volver a iniciar sesion</t>
+          <t>Error autenticacion</t>
         </is>
       </c>
     </row>

</xml_diff>